<commit_message>
Modified to allow variable section widths
</commit_message>
<xml_diff>
--- a/SetupGA.xlsx
+++ b/SetupGA.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kotab\Documents\GitHub\Seismic-DnA-GA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4101DB03-9397-4293-A56C-8F261A65CBDA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB6D1459-D9D4-4E5C-A042-B27765CCB76F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="6310" tabRatio="569" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,6 +22,13 @@
     <definedName name="solver_opt" localSheetId="0">#REF!</definedName>
   </definedNames>
   <calcPr calcId="179021"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -2068,12 +2075,6 @@
     <t>Member property col</t>
   </si>
   <si>
-    <t>Material properties cols</t>
-  </si>
-  <si>
-    <t>Section properties cols</t>
-  </si>
-  <si>
     <t>Variables to multiply</t>
   </si>
   <si>
@@ -2147,6 +2148,12 @@
   </si>
   <si>
     <t>AG,AJ,AM</t>
+  </si>
+  <si>
+    <t>Section property defs</t>
+  </si>
+  <si>
+    <t>Material property defs</t>
   </si>
 </sst>
 </file>
@@ -2651,10 +2658,10 @@
   <dimension ref="A1:AQ1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="I4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="K7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="M7" sqref="M7"/>
+      <selection pane="bottomRight" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2817,14 +2824,14 @@
       <c r="AK3" s="17"/>
       <c r="AL3" s="17"/>
       <c r="AM3" s="30" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="AN3" s="17"/>
       <c r="AO3" s="17"/>
     </row>
     <row r="4" spans="1:42" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="18" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="B4" s="10">
         <v>4</v>
@@ -2884,7 +2891,7 @@
         <v>19</v>
       </c>
       <c r="W4" s="10" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="Z4" s="10" t="s">
         <v>436</v>
@@ -2915,7 +2922,7 @@
         <v>5</v>
       </c>
       <c r="AM4" s="10" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="AP4" s="9" t="s">
         <v>44</v>
@@ -2923,10 +2930,10 @@
     </row>
     <row r="5" spans="1:42" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
+        <v>680</v>
+      </c>
+      <c r="B5" s="10" t="s">
         <v>682</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>684</v>
       </c>
       <c r="C5" s="1">
         <v>2</v>
@@ -2984,7 +2991,7 @@
         <v>19</v>
       </c>
       <c r="W5" s="10" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="Z5" s="10" t="s">
         <v>5</v>
@@ -3083,10 +3090,10 @@
         <v>19</v>
       </c>
       <c r="W6" s="10" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="Z6" s="10" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="AA6" s="19">
         <v>1250000000</v>
@@ -3183,7 +3190,7 @@
         <v>19</v>
       </c>
       <c r="W7" s="10" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="Z7" s="10" t="s">
         <v>437</v>
@@ -3282,7 +3289,7 @@
         <v>19</v>
       </c>
       <c r="W8" s="10" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="Z8" s="10" t="s">
         <v>449</v>
@@ -3376,10 +3383,10 @@
         <v>19</v>
       </c>
       <c r="W9" s="10" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="Z9" s="10" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="AA9" s="10">
         <v>1962</v>
@@ -3399,7 +3406,7 @@
         <v>671</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="C10" s="1">
         <v>7</v>
@@ -3457,7 +3464,7 @@
         <v>19</v>
       </c>
       <c r="W10" s="10" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="AI10" s="19"/>
       <c r="AP10" s="9" t="s">
@@ -3527,7 +3534,7 @@
         <v>19</v>
       </c>
       <c r="W11" s="10" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="AP11" s="9" t="s">
         <v>90</v>
@@ -3596,7 +3603,7 @@
         <v>19</v>
       </c>
       <c r="W12" s="10" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="AP12" s="9" t="s">
         <v>100</v>
@@ -3666,7 +3673,7 @@
         <v>19</v>
       </c>
       <c r="W13" s="10" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="AP13" s="9" t="s">
         <v>119</v>
@@ -3735,7 +3742,7 @@
         <v>19</v>
       </c>
       <c r="W14" s="10" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="AP14" s="9" t="s">
         <v>122</v>
@@ -3804,7 +3811,7 @@
         <v>19</v>
       </c>
       <c r="W15" s="10" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="16" spans="1:42" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -3870,7 +3877,7 @@
         <v>19</v>
       </c>
       <c r="W16" s="10" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="17" spans="1:43" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -3936,7 +3943,7 @@
         <v>19</v>
       </c>
       <c r="W17" s="10" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="18" spans="1:43" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -4002,12 +4009,12 @@
         <v>19</v>
       </c>
       <c r="W18" s="10" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="19" spans="1:43" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="10" t="s">
-        <v>680</v>
+        <v>706</v>
       </c>
       <c r="B19" s="10" t="s">
         <v>668</v>
@@ -4068,15 +4075,15 @@
         <v>19</v>
       </c>
       <c r="W19" s="10" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="20" spans="1:43" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="10" t="s">
-        <v>681</v>
+        <v>705</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="C20" s="1">
         <v>17</v>
@@ -4134,15 +4141,15 @@
         <v>19</v>
       </c>
       <c r="W20" s="10" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="21" spans="1:43" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="10" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="C21" s="1">
         <v>18</v>
@@ -4200,15 +4207,15 @@
         <v>19</v>
       </c>
       <c r="W21" s="10" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="22" spans="1:43" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="10" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="B22" s="10">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C22" s="1">
         <v>19</v>
@@ -4266,15 +4273,15 @@
         <v>19</v>
       </c>
       <c r="W22" s="10" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="23" spans="1:43" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="10" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="B23" s="10">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="C23" s="1">
         <v>20</v>
@@ -4332,12 +4339,12 @@
         <v>19</v>
       </c>
       <c r="W23" s="10" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="24" spans="1:43" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="10" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="B24" s="10">
         <v>23</v>
@@ -4398,7 +4405,7 @@
         <v>19</v>
       </c>
       <c r="W24" s="10" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="AP24" t="s">
         <v>143</v>
@@ -4406,10 +4413,10 @@
     </row>
     <row r="25" spans="1:43" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="10" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="C25" s="1">
         <v>22</v>
@@ -4467,15 +4474,15 @@
         <v>19</v>
       </c>
       <c r="W25" s="10" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="26" spans="1:43" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="10" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="C26" s="1">
         <v>23</v>
@@ -4533,7 +4540,7 @@
         <v>19</v>
       </c>
       <c r="W26" s="10" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="AP26" t="s">
         <v>149</v>
@@ -4545,10 +4552,10 @@
     </row>
     <row r="27" spans="1:43" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="10" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="C27" s="1">
         <v>24</v>
@@ -4591,7 +4598,7 @@
         <v>19</v>
       </c>
       <c r="W27" s="10" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="AP27" t="s">
         <v>152</v>
@@ -4603,10 +4610,10 @@
     </row>
     <row r="28" spans="1:43" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="10" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="B28" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C28" s="1">
         <v>25</v>
@@ -4650,7 +4657,7 @@
         <v>19</v>
       </c>
       <c r="W28" s="10" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="AP28" t="s">
         <v>154</v>
@@ -4662,7 +4669,7 @@
     </row>
     <row r="29" spans="1:43" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="18" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="B29" s="10">
         <v>0.01</v>
@@ -4709,7 +4716,7 @@
         <v>19</v>
       </c>
       <c r="W29" s="10" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="AP29" t="s">
         <v>157</v>
@@ -4721,7 +4728,7 @@
     </row>
     <row r="30" spans="1:43" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="18" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="B30" s="10">
         <v>0</v>
@@ -4768,7 +4775,7 @@
         <v>19</v>
       </c>
       <c r="W30" s="10" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="AP30" t="s">
         <v>159</v>
@@ -4780,7 +4787,7 @@
     </row>
     <row r="31" spans="1:43" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="18" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="B31" s="10">
         <v>3</v>
@@ -4813,6 +4820,12 @@
         <v>0</v>
       </c>
       <c r="M31" s="1"/>
+      <c r="O31">
+        <v>2</v>
+      </c>
+      <c r="P31">
+        <v>6</v>
+      </c>
       <c r="S31" s="1">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -4827,7 +4840,7 @@
         <v>19</v>
       </c>
       <c r="W31" s="10" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="AP31" t="s">
         <v>162</v>
@@ -4838,10 +4851,10 @@
     </row>
     <row r="32" spans="1:43" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="18" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="B32" s="10">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C32" s="1">
         <v>29</v>
@@ -4885,7 +4898,7 @@
         <v>19</v>
       </c>
       <c r="W32" s="10" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="AP32" t="s">
         <v>165</v>
@@ -4938,7 +4951,7 @@
         <v>19</v>
       </c>
       <c r="W33" s="10" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="34" spans="3:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -4984,7 +4997,7 @@
         <v>19</v>
       </c>
       <c r="W34" s="10" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="35" spans="3:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -5030,7 +5043,7 @@
         <v>19</v>
       </c>
       <c r="W35" s="10" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="36" spans="3:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -5076,7 +5089,7 @@
         <v>19</v>
       </c>
       <c r="W36" s="10" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="37" spans="3:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -5122,7 +5135,7 @@
         <v>19</v>
       </c>
       <c r="W37" s="10" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="38" spans="3:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -5168,7 +5181,7 @@
         <v>19</v>
       </c>
       <c r="W38" s="10" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="39" spans="3:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -5214,7 +5227,7 @@
         <v>19</v>
       </c>
       <c r="W39" s="10" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="40" spans="3:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -5260,7 +5273,7 @@
         <v>19</v>
       </c>
       <c r="W40" s="10" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="41" spans="3:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -5306,7 +5319,7 @@
         <v>19</v>
       </c>
       <c r="W41" s="10" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="42" spans="3:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -5352,7 +5365,7 @@
         <v>19</v>
       </c>
       <c r="W42" s="10" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="43" spans="3:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -5398,7 +5411,7 @@
         <v>19</v>
       </c>
       <c r="W43" s="10" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="44" spans="3:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -5444,7 +5457,7 @@
         <v>19</v>
       </c>
       <c r="W44" s="10" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="45" spans="3:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -5490,7 +5503,7 @@
         <v>19</v>
       </c>
       <c r="W45" s="10" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="46" spans="3:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -5536,7 +5549,7 @@
         <v>19</v>
       </c>
       <c r="W46" s="10" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="47" spans="3:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -5583,7 +5596,7 @@
         <v>19</v>
       </c>
       <c r="W47" s="10" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="48" spans="3:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>